<commit_message>
Dokumentasi akhir setelah dinyatakan lulus
</commit_message>
<xml_diff>
--- a/tugas_akhir/dokumenTA/DIPAKAI_data-pengujianbsf-3.xlsx
+++ b/tugas_akhir/dokumenTA/DIPAKAI_data-pengujianbsf-3.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benny\OneDrive\Documents\PlatformIO\Projects\Project-Tugas-Akhir\tugas_akhir\dokumenTA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA4B3F8-6160-4C0B-8775-43117C7F90BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8648722E-656A-415B-A364-8148EAC3F313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BH1750 kalibrasi 3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sensor Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Produksi Telur Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Uji ulang fungsionalitas " sheetId="4" r:id="rId1"/>
+    <sheet name="BH1750 kalibrasi 3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sensor Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Produksi Telur Data" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Sensor Data'!$A$2:$B$21</definedName>
@@ -36,7 +37,7 @@
     <definedName name="_xlchart.v1.22" hidden="1">'Sensor Data'!$M$2:$M$21</definedName>
     <definedName name="_xlchart.v1.23" hidden="1">'Sensor Data'!$N$1</definedName>
     <definedName name="_xlchart.v1.24" hidden="1">'Sensor Data'!$N$2:$N$21</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'Sensor Data'!$P$18</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'Sensor Data'!$R$18</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Sensor Data'!$D$1</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Sensor Data'!$D$2:$D$21</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Sensor Data'!$E$1</definedName>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>tanggal</t>
   </si>
@@ -251,6 +252,30 @@
   <si>
     <t>% Mini light meter</t>
   </si>
+  <si>
+    <t>bh1750-revTA</t>
+  </si>
+  <si>
+    <t>bh1750-percent</t>
+  </si>
+  <si>
+    <t>Jam</t>
+  </si>
+  <si>
+    <t>Temperatur</t>
+  </si>
+  <si>
+    <t>Kelembapan</t>
+  </si>
+  <si>
+    <t>Intensitas cahaya</t>
+  </si>
+  <si>
+    <t>Kondisi water pump</t>
+  </si>
+  <si>
+    <t>Kondisi lampu fertilizer</t>
+  </si>
 </sst>
 </file>
 
@@ -260,7 +285,7 @@
     <numFmt numFmtId="164" formatCode="[$-13809]hh:mm;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +319,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -316,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -333,6 +364,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3206,7 +3241,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sensor Data'!$P$17</c:f>
+              <c:f>'Sensor Data'!$R$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3240,7 +3275,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$P$18</c:f>
+              <c:f>'Sensor Data'!$R$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3261,7 +3296,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sensor Data'!$Q$17</c:f>
+              <c:f>'Sensor Data'!$S$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3285,7 +3320,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$Q$18</c:f>
+              <c:f>'Sensor Data'!$S$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3306,7 +3341,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sensor Data'!$R$17</c:f>
+              <c:f>'Sensor Data'!$T$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3330,7 +3365,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$R$18</c:f>
+              <c:f>'Sensor Data'!$T$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3690,7 +3725,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sensor Data'!$T$8</c:f>
+              <c:f>'Sensor Data'!$V$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3711,7 +3746,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$T$9</c:f>
+              <c:f>'Sensor Data'!$V$9</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3732,7 +3767,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sensor Data'!$U$8</c:f>
+              <c:f>'Sensor Data'!$W$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3753,7 +3788,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$U$9</c:f>
+              <c:f>'Sensor Data'!$W$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3774,7 +3809,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sensor Data'!$V$8</c:f>
+              <c:f>'Sensor Data'!$X$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3795,7 +3830,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$V$9</c:f>
+              <c:f>'Sensor Data'!$X$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3833,7 +3868,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$P$17</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$R$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3873,7 +3908,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$P$18</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$R$18</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3902,7 +3937,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$Q$17</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$S$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3932,7 +3967,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$Q$18</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$S$18</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3961,7 +3996,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$R$17</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$T$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -3991,7 +4026,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$R$18</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$T$18</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4020,7 +4055,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$P$8</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$R$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4047,7 +4082,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$P$9</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$R$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4076,7 +4111,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$Q$8</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$S$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4103,7 +4138,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$Q$9</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$S$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4132,7 +4167,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$R$8</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$T$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4159,7 +4194,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Sensor Data'!$R$9</c15:sqref>
+                          <c15:sqref>'Sensor Data'!$T$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -4383,7 +4418,7 @@
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>Perbandingan </a:t>
+              <a:t> </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-ID" sz="1400" i="1">
@@ -4558,9 +4593,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sensor Data'!$P$8:$W$8</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sensor Data'!$R$8:$Y$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sensor Data'!$R$8:$T$8</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>avg-dht11-temp</c:v>
                 </c:pt>
@@ -4570,24 +4612,22 @@
                 <c:pt idx="2">
                   <c:v>max-dht11-temp</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>avg-alat ukur-temp</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>min-alat ukur-temp</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>max-alat ukur-temp</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$P$9:$W$9</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sensor Data'!$R$9:$Y$9</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sensor Data'!$R$9:$T$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="0.0">
                   <c:v>31.985000000000003</c:v>
                 </c:pt>
@@ -4596,15 +4636,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>36.1</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.0">
-                  <c:v>32.105000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35.200000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4830,13 +4861,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-ID" sz="1400">
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:rPr>
-              <a:t>Perbandingan </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-ID" sz="1400" i="1">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -4995,9 +5019,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sensor Data'!$P$11:$W$11</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sensor Data'!$R$11:$Y$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sensor Data'!$R$11:$T$11</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>avg-dht11-humi</c:v>
                 </c:pt>
@@ -5007,24 +5038,22 @@
                 <c:pt idx="2">
                   <c:v>max-dht11-humi</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>avg-alat ukur-humi</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>min-alat ukur-humi</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>max-alat ukur-humi</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$P$12:$W$12</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sensor Data'!$R$12:$Y$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sensor Data'!$R$12:$T$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>60.8</c:v>
                 </c:pt>
@@ -5033,15 +5062,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.0">
-                  <c:v>64.349999999999994</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5267,13 +5287,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-ID" sz="1400">
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              </a:rPr>
-              <a:t>Perbandingan </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-ID" sz="1400" i="1">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -5446,9 +5459,16 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sensor Data'!$P$14:$W$14</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sensor Data'!$R$14:$Y$14</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sensor Data'!$R$14:$T$14</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>avg-bh1750-lx</c:v>
                 </c:pt>
@@ -5458,41 +5478,30 @@
                 <c:pt idx="2">
                   <c:v>max-bh1750-lx</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>avg-alat ukur-lx</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>min-alat ukur-lx</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>max-alat ukur-lx</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$P$15:$W$15</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Sensor Data'!$R$15:$Y$15</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Sensor Data'!$R$15:$T$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5640.7</c:v>
+                  <c:v>15004.261999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2100</c:v>
+                  <c:v>5586</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17355</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14813.9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4905</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>46520</c:v>
+                  <c:v>46164.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5588,7 +5597,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5957,7 +5966,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sensor Data'!$P$17:$R$17</c:f>
+              <c:f>'Sensor Data'!$R$17:$T$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -5974,7 +5983,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$P$18:$R$18</c:f>
+              <c:f>'Sensor Data'!$R$18:$T$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6419,7 +6428,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sensor Data'!$P$20:$R$20</c:f>
+              <c:f>'Sensor Data'!$R$20:$T$20</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -6436,7 +6445,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$P$21:$R$21</c:f>
+              <c:f>'Sensor Data'!$R$21:$T$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6847,7 +6856,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sensor Data'!$T$17:$V$17</c:f>
+              <c:f>'Sensor Data'!$V$17:$X$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -6864,18 +6873,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sensor Data'!$T$18:$V$18</c:f>
+              <c:f>'Sensor Data'!$V$18:$X$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.5865660135161903</c:v>
+                  <c:v>5.4295957763310164E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77883981542518133</c:v>
+                  <c:v>3.4768619160633197E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8122974349476804</c:v>
+                  <c:v>0.33126322728376639</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -47285,7 +47294,7 @@
       <xdr:rowOff>574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>175107</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>574</xdr:rowOff>
@@ -47321,7 +47330,7 @@
       <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>171176</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>159840</xdr:rowOff>
@@ -47351,13 +47360,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>317699</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>31195</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>28332</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>25795</xdr:rowOff>
@@ -47387,13 +47396,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>329754</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>35388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>24953</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>35389</xdr:rowOff>
@@ -47465,7 +47474,7 @@
       <xdr:rowOff>118069</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>167633</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>118069</xdr:rowOff>
@@ -47495,13 +47504,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304588</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>135097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>607383</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>135097</xdr:rowOff>
@@ -47531,13 +47540,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>343547</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>102991</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>36742</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>102989</xdr:rowOff>
@@ -47567,13 +47576,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>10391</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>51954</xdr:rowOff>
@@ -47603,13 +47612,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>411079</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>72190</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>90237</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>108284</xdr:rowOff>
@@ -47639,13 +47648,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>441158</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>122321</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>120316</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>158415</xdr:rowOff>
@@ -47675,13 +47684,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>273538</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>5862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>150447</xdr:rowOff>
@@ -47711,13 +47720,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>283308</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>64478</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>9770</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>23447</xdr:rowOff>
@@ -47747,13 +47756,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>410307</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>132862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>136769</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>91831</xdr:rowOff>
@@ -47783,13 +47792,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>603449</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>31195</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>314082</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>25795</xdr:rowOff>
@@ -47819,13 +47828,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>32</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -48195,6 +48204,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F376F0F0-7395-45E5-8F4C-A682BE6CAFE0}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="14"/>
+    <col min="2" max="3" width="11.88671875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="14" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="15">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15">
+        <v>0.41666666666666702</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15">
+        <v>0.45833333333333298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="15">
+        <v>0.47916666666666702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15">
+        <v>0.52083333333333304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15">
+        <v>0.54166666666666696</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="15">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB8897A-43C1-4EF5-95E8-63379DB3A574}">
   <dimension ref="A1:I14"/>
   <sheetViews>
@@ -48656,17 +48763,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AO14" sqref="AO14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -48712,14 +48824,20 @@
       <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="P1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:24">
       <c r="A2" s="1">
         <v>45082</v>
       </c>
@@ -48771,15 +48889,23 @@
       <c r="O2">
         <v>3</v>
       </c>
-      <c r="T2">
+      <c r="P2" s="12">
+        <f>G2+(1.66*G2)</f>
+        <v>13613.88</v>
+      </c>
+      <c r="Q2" s="5">
+        <f>ABS(((P2-H2)/P2)*100%)</f>
+        <v>1.5874974658216526E-2</v>
+      </c>
+      <c r="V2">
         <f>AVERAGE(O2:O21)</f>
         <v>3.3</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:24">
       <c r="A3" s="1"/>
       <c r="B3" s="2">
         <v>0.58333333333333337</v>
@@ -48829,11 +48955,19 @@
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="U3" t="s">
+      <c r="P3" s="12">
+        <f t="shared" ref="P3:P21" si="6">G3+(1.66*G3)</f>
+        <v>8070.44</v>
+      </c>
+      <c r="Q3" s="5">
+        <f t="shared" ref="Q3:Q21" si="7">ABS(((P3-H3)/P3)*100%)</f>
+        <v>0.33126322728376639</v>
+      </c>
+      <c r="W3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:24">
       <c r="A4" s="1">
         <v>45083</v>
       </c>
@@ -48885,11 +49019,19 @@
       <c r="O4">
         <v>3</v>
       </c>
-      <c r="U4" t="s">
+      <c r="P4" s="12">
+        <f t="shared" si="6"/>
+        <v>10520.3</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" si="7"/>
+        <v>7.0939041662309951E-2</v>
+      </c>
+      <c r="W4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:24">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
         <v>0.58333333333333337</v>
@@ -48939,14 +49081,22 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="T5" t="s">
+      <c r="P5" s="12">
+        <f t="shared" si="6"/>
+        <v>5586</v>
+      </c>
+      <c r="Q5" s="5">
+        <f t="shared" si="7"/>
+        <v>0.12191192266380237</v>
+      </c>
+      <c r="V5" t="s">
         <v>22</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:24">
       <c r="A6" s="1">
         <v>45084</v>
       </c>
@@ -48998,11 +49148,19 @@
       <c r="O6">
         <v>3</v>
       </c>
-      <c r="U6" t="s">
+      <c r="P6" s="12">
+        <f t="shared" si="6"/>
+        <v>20482</v>
+      </c>
+      <c r="Q6" s="5">
+        <f t="shared" si="7"/>
+        <v>3.3590469680695248E-2</v>
+      </c>
+      <c r="W6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:24">
       <c r="A7" s="1"/>
       <c r="B7" s="2">
         <v>0.58333333333333337</v>
@@ -49052,8 +49210,16 @@
       <c r="O7">
         <v>2</v>
       </c>
+      <c r="P7" s="12">
+        <f t="shared" si="6"/>
+        <v>7418.74</v>
+      </c>
+      <c r="Q7" s="5">
+        <f t="shared" si="7"/>
+        <v>4.7547157603582253E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:24">
       <c r="A8" s="1">
         <v>45085</v>
       </c>
@@ -49105,26 +49271,34 @@
       <c r="O8">
         <v>4</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="12">
+        <f t="shared" si="6"/>
+        <v>12613.72</v>
+      </c>
+      <c r="Q8" s="5">
+        <f t="shared" si="7"/>
+        <v>2.2695921583799281E-2</v>
+      </c>
+      <c r="R8" t="s">
         <v>45</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="S8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="T8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="T8" s="5" t="s">
+      <c r="V8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="W8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="V8" s="5" t="s">
+      <c r="X8" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:24">
       <c r="A9" s="1"/>
       <c r="B9" s="2">
         <v>0.58333333333333337</v>
@@ -49174,32 +49348,40 @@
       <c r="O9">
         <v>4</v>
       </c>
-      <c r="P9" s="8">
+      <c r="P9" s="12">
+        <f t="shared" si="6"/>
+        <v>15348.199999999999</v>
+      </c>
+      <c r="Q9" s="5">
+        <f t="shared" si="7"/>
+        <v>1.7708917006554588E-2</v>
+      </c>
+      <c r="R9" s="8">
         <f>AVERAGE(C2:C21)</f>
         <v>31.985000000000003</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="S9" s="7">
         <f>MIN(C2:C21)</f>
         <v>28.1</v>
       </c>
-      <c r="R9" s="7">
+      <c r="T9" s="7">
         <f>MAX(C2:C21)</f>
         <v>36.1</v>
       </c>
-      <c r="T9" s="8">
+      <c r="V9" s="8">
         <f>AVERAGE(D2:D21)</f>
         <v>32.105000000000004</v>
       </c>
-      <c r="U9" s="7">
+      <c r="W9" s="7">
         <f>MIN(D2:D21)</f>
         <v>29.5</v>
       </c>
-      <c r="V9" s="7">
+      <c r="X9" s="7">
         <f>MAX(D2:D21)</f>
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:24">
       <c r="A10" s="1">
         <v>45086</v>
       </c>
@@ -49251,8 +49433,16 @@
       <c r="O10">
         <v>4</v>
       </c>
+      <c r="P10" s="12">
+        <f t="shared" si="6"/>
+        <v>8692.880000000001</v>
+      </c>
+      <c r="Q10" s="5">
+        <f t="shared" si="7"/>
+        <v>2.1985809075933289E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:24">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>0.58333333333333337</v>
@@ -49302,26 +49492,34 @@
       <c r="O11">
         <v>4</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="12">
+        <f t="shared" si="6"/>
+        <v>17300.64</v>
+      </c>
+      <c r="Q11" s="5">
+        <f t="shared" si="7"/>
+        <v>2.9515671096560558E-2</v>
+      </c>
+      <c r="R11" t="s">
         <v>46</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="S11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R11" s="5" t="s">
+      <c r="T11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="T11" s="5" t="s">
+      <c r="V11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="U11" s="5" t="s">
+      <c r="W11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="V11" s="5" t="s">
+      <c r="X11" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:24">
       <c r="A12" s="1">
         <v>45089</v>
       </c>
@@ -49373,32 +49571,40 @@
       <c r="O12">
         <v>5</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="12">
+        <f t="shared" si="6"/>
+        <v>12613.72</v>
+      </c>
+      <c r="Q12" s="5">
+        <f t="shared" si="7"/>
+        <v>2.2695921583799281E-2</v>
+      </c>
+      <c r="R12">
         <f>AVERAGE(E2:E21)</f>
         <v>60.8</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="S12" s="7">
         <f>MIN(E2:E21)</f>
         <v>46</v>
       </c>
-      <c r="R12" s="7">
+      <c r="T12" s="7">
         <f>MAX(E2:E21)</f>
         <v>82</v>
       </c>
-      <c r="T12" s="8">
+      <c r="V12" s="8">
         <f>AVERAGE(F2:F21)</f>
         <v>64.349999999999994</v>
       </c>
-      <c r="U12" s="7">
+      <c r="W12" s="7">
         <f>MIN(F2:F21)</f>
         <v>48</v>
       </c>
-      <c r="V12" s="7">
+      <c r="X12" s="7">
         <f>MAX(F2:F21)</f>
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:24">
       <c r="A13" s="1"/>
       <c r="B13" s="2">
         <v>0.58333333333333337</v>
@@ -49448,8 +49654,16 @@
       <c r="O13">
         <v>3</v>
       </c>
+      <c r="P13" s="12">
+        <f t="shared" si="6"/>
+        <v>28725.34</v>
+      </c>
+      <c r="Q13" s="5">
+        <f t="shared" si="7"/>
+        <v>5.7254674792361022E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:24">
       <c r="A14" s="1">
         <v>45090</v>
       </c>
@@ -49501,26 +49715,34 @@
       <c r="O14">
         <v>3</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="12">
+        <f t="shared" si="6"/>
+        <v>8259.2999999999993</v>
+      </c>
+      <c r="Q14" s="5">
+        <f t="shared" si="7"/>
+        <v>4.1250469168089395E-2</v>
+      </c>
+      <c r="R14" t="s">
         <v>47</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="S14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="R14" s="5" t="s">
+      <c r="T14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="V14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="W14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V14" s="5" t="s">
+      <c r="X14" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:24">
       <c r="A15" s="1"/>
       <c r="B15" s="2">
         <v>0.58333333333333337</v>
@@ -49570,32 +49792,40 @@
       <c r="O15">
         <v>4</v>
       </c>
-      <c r="P15">
-        <f>AVERAGE(G2:G21)</f>
-        <v>5640.7</v>
-      </c>
-      <c r="Q15" s="7">
-        <f>MIN(G2:G21)</f>
-        <v>2100</v>
-      </c>
-      <c r="R15" s="7">
-        <f>MAX(G2:G21)</f>
-        <v>17355</v>
-      </c>
-      <c r="T15">
+      <c r="P15" s="12">
+        <f t="shared" si="6"/>
+        <v>8605.0999999999985</v>
+      </c>
+      <c r="Q15" s="5">
+        <f t="shared" si="7"/>
+        <v>7.3328607453717626E-3</v>
+      </c>
+      <c r="R15" s="12">
+        <f>AVERAGE(P2:P21)</f>
+        <v>15004.261999999999</v>
+      </c>
+      <c r="S15" s="13">
+        <f>MIN(P2:P21)</f>
+        <v>5586</v>
+      </c>
+      <c r="T15" s="13">
+        <f>MAX(P2:P21)</f>
+        <v>46164.3</v>
+      </c>
+      <c r="V15">
         <f>AVERAGE(H2:H21)</f>
         <v>14813.9</v>
       </c>
-      <c r="U15" s="7">
+      <c r="W15" s="7">
         <f>MIN(H2:H21)</f>
         <v>4905</v>
       </c>
-      <c r="V15" s="7">
+      <c r="X15" s="7">
         <f>MAX(H2:H21)</f>
         <v>46520</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:24">
       <c r="A16" s="1">
         <v>45091</v>
       </c>
@@ -49647,8 +49877,16 @@
       <c r="O16">
         <v>4</v>
       </c>
+      <c r="P16" s="12">
+        <f t="shared" si="6"/>
+        <v>15042.3</v>
+      </c>
+      <c r="Q16" s="5">
+        <f t="shared" si="7"/>
+        <v>3.4768619160633197E-3</v>
+      </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:24">
       <c r="A17" s="1"/>
       <c r="B17" s="2">
         <v>0.58333333333333337</v>
@@ -49698,26 +49936,34 @@
       <c r="O17">
         <v>4</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="12">
+        <f t="shared" si="6"/>
+        <v>18178.439999999999</v>
+      </c>
+      <c r="Q17" s="5">
+        <f t="shared" si="7"/>
+        <v>0.16879556221545958</v>
+      </c>
+      <c r="R17" t="s">
         <v>23</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="S17" t="s">
         <v>28</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>27</v>
       </c>
-      <c r="T17" t="s">
+      <c r="V17" t="s">
         <v>25</v>
       </c>
-      <c r="U17" s="5" t="s">
+      <c r="W17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="V17" s="5" t="s">
+      <c r="X17" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:24">
       <c r="A18" s="1">
         <v>45092</v>
       </c>
@@ -49769,32 +50015,40 @@
       <c r="O18">
         <v>3</v>
       </c>
-      <c r="P18" s="5">
+      <c r="P18" s="12">
+        <f t="shared" si="6"/>
+        <v>9586.64</v>
+      </c>
+      <c r="Q18" s="5">
+        <f t="shared" si="7"/>
+        <v>3.8244890806372146E-2</v>
+      </c>
+      <c r="R18" s="5">
         <f>AVERAGE(L2:L21)</f>
         <v>3.473173876648479E-2</v>
       </c>
-      <c r="Q18" s="5">
+      <c r="S18" s="5">
         <f>MIN(L2:L21)</f>
         <v>6.3492063492063266E-3</v>
       </c>
-      <c r="R18" s="5">
+      <c r="T18" s="5">
         <f>MAX(L2:L21)</f>
         <v>6.7901234567901217E-2</v>
       </c>
-      <c r="T18" s="5">
-        <f>AVERAGE(N2:N21)</f>
-        <v>1.5865660135161903</v>
-      </c>
-      <c r="U18" s="5">
-        <f>MIN(N2:N21)</f>
-        <v>0.77883981542518133</v>
-      </c>
       <c r="V18" s="5">
-        <f>MAX(N2:N21)</f>
-        <v>1.8122974349476804</v>
+        <f>AVERAGE(Q2:Q21)</f>
+        <v>5.4295957763310164E-2</v>
+      </c>
+      <c r="W18" s="5">
+        <f>MIN(Q2:Q21)</f>
+        <v>3.4768619160633197E-3</v>
+      </c>
+      <c r="X18" s="5">
+        <f>MAX(Q2:Q21)</f>
+        <v>0.33126322728376639</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:24">
       <c r="A19" s="1"/>
       <c r="B19" s="2">
         <v>0.58333333333333337</v>
@@ -49844,8 +50098,16 @@
       <c r="O19">
         <v>3</v>
       </c>
+      <c r="P19" s="12">
+        <f t="shared" si="6"/>
+        <v>22570.1</v>
+      </c>
+      <c r="Q19" s="5">
+        <f t="shared" si="7"/>
+        <v>1.2401362865029462E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:24">
       <c r="A20" s="1">
         <v>45093</v>
       </c>
@@ -49897,17 +50159,25 @@
       <c r="O20">
         <v>4</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P20" s="12">
+        <f t="shared" si="6"/>
+        <v>10693.2</v>
+      </c>
+      <c r="Q20" s="5">
+        <f t="shared" si="7"/>
+        <v>1.3728350727565113E-2</v>
+      </c>
+      <c r="R20" t="s">
         <v>24</v>
       </c>
-      <c r="Q20" s="5" t="s">
+      <c r="S20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R20" s="5" t="s">
+      <c r="T20" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:24">
       <c r="B21" s="2">
         <v>0.58333333333333337</v>
       </c>
@@ -49956,27 +50226,41 @@
       <c r="O21">
         <v>3</v>
       </c>
-      <c r="P21" s="5">
+      <c r="P21" s="12">
+        <f t="shared" si="6"/>
+        <v>46164.3</v>
+      </c>
+      <c r="Q21" s="5">
+        <f t="shared" si="7"/>
+        <v>7.7050881308716275E-3</v>
+      </c>
+      <c r="R21" s="5">
         <f>AVERAGE(M2:M21)</f>
         <v>7.3299866060484581E-2</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="S21" s="5">
         <f>MIN(M2:M21)</f>
         <v>0</v>
       </c>
-      <c r="R21" s="5">
+      <c r="T21" s="5">
         <f>MAX(M2:M21)</f>
         <v>0.21666666666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:24">
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:24">
       <c r="E23" s="3"/>
+      <c r="F23">
+        <f>AVERAGE(F2:F21)</f>
+        <v>64.349999999999994</v>
+      </c>
       <c r="H23" t="s">
         <v>51</v>
       </c>
@@ -49985,82 +50269,114 @@
         <v>1.119999999999999</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23:N23" si="6">AVERAGE(J2:J21)</f>
+        <f t="shared" ref="J23:N23" si="8">AVERAGE(J2:J21)</f>
         <v>4.3499999999999996</v>
       </c>
       <c r="K23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9173.2000000000007</v>
       </c>
       <c r="L23" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.473173876648479E-2</v>
       </c>
       <c r="M23" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.3299866060484581E-2</v>
       </c>
       <c r="N23" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1.5865660135161903</v>
       </c>
+      <c r="P23" s="12">
+        <f>AVERAGE(P2:P21)</f>
+        <v>15004.261999999999</v>
+      </c>
+      <c r="Q23" s="5">
+        <f>AVERAGE(Q2:Q22)</f>
+        <v>5.4295957763310164E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:24">
+      <c r="F24">
+        <f>MAX(F2:F21)</f>
+        <v>79</v>
+      </c>
       <c r="H24" t="s">
         <v>52</v>
       </c>
       <c r="I24" s="9">
-        <f t="shared" ref="I24:N24" si="7">MAX(I2:I21)</f>
+        <f t="shared" ref="I24:N24" si="9">MAX(I2:I21)</f>
         <v>2.3999999999999986</v>
       </c>
       <c r="J24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="K24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>29165</v>
       </c>
       <c r="L24" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6.7901234567901217E-2</v>
       </c>
       <c r="M24" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.21666666666666667</v>
       </c>
       <c r="N24" s="10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.8122974349476804</v>
       </c>
+      <c r="P24" s="12">
+        <f>MAX(P2:P21)</f>
+        <v>46164.3</v>
+      </c>
+      <c r="Q24" s="5">
+        <f>MAX(Q2:Q22)</f>
+        <v>0.33126322728376639</v>
+      </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:24">
+      <c r="F25">
+        <f>MIN(F2:F21)</f>
+        <v>48</v>
+      </c>
       <c r="H25" t="s">
         <v>53</v>
       </c>
       <c r="I25" s="9">
-        <f t="shared" ref="I25:N25" si="8">MIN(I2:I21)</f>
+        <f t="shared" ref="I25:N25" si="10">MIN(I2:I21)</f>
         <v>0.19999999999999929</v>
       </c>
       <c r="J25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2363</v>
       </c>
       <c r="L25" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.3492063492063266E-3</v>
       </c>
       <c r="M25" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N25" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.77883981542518133</v>
+      </c>
+      <c r="P25" s="12">
+        <f>MIN(P2:P21)</f>
+        <v>5586</v>
+      </c>
+      <c r="Q25" s="5">
+        <f>MIN(Q2:Q21)</f>
+        <v>3.4768619160633197E-3</v>
       </c>
     </row>
   </sheetData>
@@ -50071,7 +50387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302D2EB0-8602-40F5-B743-D70D0FC2E10C}">
   <dimension ref="A1:G7"/>
   <sheetViews>

</xml_diff>